<commit_message>
corrected the error in this chart
</commit_message>
<xml_diff>
--- a/FrenchData/Accounts/q2_output/merged_TOP3_monthlyFr.xlsx
+++ b/FrenchData/Accounts/q2_output/merged_TOP3_monthlyFr.xlsx
@@ -8,16 +8,13 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\brieh\Projects\KEY_RA\Environment_Canada\ECCC\FrenchData\Accounts\q2_output\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{A0A8ABAC-5A50-47BF-98CC-718D33B905EB}" xr6:coauthVersionLast="28" xr6:coauthVersionMax="28" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{FBA4B579-07E0-40A8-9FCC-DA7A307E152D}" xr6:coauthVersionLast="28" xr6:coauthVersionMax="28" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="0" yWindow="0" windowWidth="16920" windowHeight="7650" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="merged_TOP3_monthly" sheetId="1" r:id="rId1"/>
   </sheets>
-  <externalReferences>
-    <externalReference r:id="rId2"/>
-  </externalReferences>
   <calcPr calcId="0"/>
 </workbook>
 </file>
@@ -1546,7 +1543,7 @@
       <scheme val="minor"/>
     </font>
   </fonts>
-  <fills count="33">
+  <fills count="34">
     <fill>
       <patternFill patternType="none"/>
     </fill>
@@ -1726,6 +1723,12 @@
         <bgColor indexed="65"/>
       </patternFill>
     </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor rgb="FFFF0000"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
   </fills>
   <borders count="10">
     <border>
@@ -1888,7 +1891,7 @@
     <xf numFmtId="0" fontId="1" fillId="32" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
     <xf numFmtId="0" fontId="19" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
   </cellStyleXfs>
-  <cellXfs count="5">
+  <cellXfs count="7">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="22" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
@@ -1898,6 +1901,8 @@
       <alignment horizontal="left" vertical="center"/>
     </xf>
     <xf numFmtId="0" fontId="19" fillId="0" borderId="0" xfId="42"/>
+    <xf numFmtId="0" fontId="0" fillId="33" borderId="0" xfId="0" applyFill="1"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyFill="1"/>
   </cellXfs>
   <cellStyles count="43">
     <cellStyle name="20% - Accent1" xfId="19" builtinId="30" customBuiltin="1"/>
@@ -2197,7 +2202,7 @@
                   <c:v>337</c:v>
                 </c:pt>
                 <c:pt idx="3">
-                  <c:v>4091</c:v>
+                  <c:v>2296</c:v>
                 </c:pt>
                 <c:pt idx="4">
                   <c:v>1789</c:v>
@@ -2357,7 +2362,7 @@
                   <c:v>155</c:v>
                 </c:pt>
                 <c:pt idx="3">
-                  <c:v>2379</c:v>
+                  <c:v>1074</c:v>
                 </c:pt>
                 <c:pt idx="4">
                   <c:v>230</c:v>
@@ -2517,7 +2522,7 @@
                   <c:v>119</c:v>
                 </c:pt>
                 <c:pt idx="3">
-                  <c:v>2214</c:v>
+                  <c:v>185</c:v>
                 </c:pt>
                 <c:pt idx="4">
                   <c:v>169</c:v>
@@ -4848,235 +4853,6 @@
 </xdr:wsDr>
 </file>
 
-<file path=xl/externalLinks/externalLink1.xml><?xml version="1.0" encoding="utf-8"?>
-<externalLink xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" mc:Ignorable="x14">
-  <externalBook xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" r:id="rId1">
-    <sheetNames>
-      <sheetName val="merged_TOP3_monthly graph"/>
-    </sheetNames>
-    <sheetDataSet>
-      <sheetData sheetId="0">
-        <row r="1">
-          <cell r="W1" t="str">
-            <v>Top 1</v>
-          </cell>
-          <cell r="X1" t="str">
-            <v>Top 2</v>
-          </cell>
-          <cell r="Y1" t="str">
-            <v>Top 3</v>
-          </cell>
-        </row>
-        <row r="2">
-          <cell r="U2" t="str">
-            <v>Marine Conservation Photo Park</v>
-          </cell>
-          <cell r="V2" t="str">
-            <v>Jan</v>
-          </cell>
-          <cell r="W2">
-            <v>6718</v>
-          </cell>
-          <cell r="X2">
-            <v>4039</v>
-          </cell>
-          <cell r="Y2">
-            <v>3086</v>
-          </cell>
-        </row>
-        <row r="3">
-          <cell r="U3" t="str">
-            <v>Photo Government Tax Money Friend</v>
-          </cell>
-          <cell r="V3" t="str">
-            <v>Feb</v>
-          </cell>
-          <cell r="W3">
-            <v>6503</v>
-          </cell>
-          <cell r="X3">
-            <v>3878</v>
-          </cell>
-          <cell r="Y3">
-            <v>3684</v>
-          </cell>
-        </row>
-        <row r="4">
-          <cell r="U4" t="str">
-            <v>Mountain Park Photo Forest</v>
-          </cell>
-          <cell r="V4" t="str">
-            <v>Mar</v>
-          </cell>
-          <cell r="W4">
-            <v>2766</v>
-          </cell>
-          <cell r="X4">
-            <v>2490</v>
-          </cell>
-          <cell r="Y4">
-            <v>2411</v>
-          </cell>
-        </row>
-        <row r="5">
-          <cell r="U5" t="str">
-            <v>Park Conservation Summer Camp</v>
-          </cell>
-          <cell r="V5" t="str">
-            <v>Apr</v>
-          </cell>
-          <cell r="W5">
-            <v>4091</v>
-          </cell>
-          <cell r="X5">
-            <v>2379</v>
-          </cell>
-          <cell r="Y5">
-            <v>2214</v>
-          </cell>
-        </row>
-        <row r="6">
-          <cell r="U6" t="str">
-            <v>Lake Park Photo</v>
-          </cell>
-          <cell r="V6" t="str">
-            <v>May</v>
-          </cell>
-          <cell r="W6">
-            <v>11478</v>
-          </cell>
-          <cell r="X6">
-            <v>9031</v>
-          </cell>
-          <cell r="Y6">
-            <v>6678</v>
-          </cell>
-        </row>
-        <row r="7">
-          <cell r="U7" t="str">
-            <v>Race Marine Conservation Photo</v>
-          </cell>
-          <cell r="V7" t="str">
-            <v>Jun</v>
-          </cell>
-          <cell r="W7">
-            <v>3481</v>
-          </cell>
-          <cell r="X7">
-            <v>3435</v>
-          </cell>
-          <cell r="Y7">
-            <v>2573</v>
-          </cell>
-        </row>
-        <row r="8">
-          <cell r="U8" t="str">
-            <v>Park Photo Video Wild</v>
-          </cell>
-          <cell r="V8" t="str">
-            <v>Jul</v>
-          </cell>
-          <cell r="W8">
-            <v>3323</v>
-          </cell>
-          <cell r="X8">
-            <v>2868</v>
-          </cell>
-          <cell r="Y8">
-            <v>2290</v>
-          </cell>
-        </row>
-        <row r="9">
-          <cell r="U9" t="str">
-            <v>Future Service Park</v>
-          </cell>
-          <cell r="V9" t="str">
-            <v>Aug</v>
-          </cell>
-          <cell r="W9">
-            <v>6442</v>
-          </cell>
-          <cell r="X9">
-            <v>4248</v>
-          </cell>
-          <cell r="Y9">
-            <v>1616</v>
-          </cell>
-        </row>
-        <row r="10">
-          <cell r="U10" t="str">
-            <v>Tree Friend Home Canada150 Mountain Park</v>
-          </cell>
-          <cell r="V10" t="str">
-            <v>Sep</v>
-          </cell>
-          <cell r="W10">
-            <v>7862</v>
-          </cell>
-          <cell r="X10">
-            <v>1749</v>
-          </cell>
-          <cell r="Y10">
-            <v>1678</v>
-          </cell>
-        </row>
-        <row r="11">
-          <cell r="U11" t="str">
-            <v>Northern Summer Job Park Natural Photo</v>
-          </cell>
-          <cell r="V11" t="str">
-            <v>Oct</v>
-          </cell>
-          <cell r="W11">
-            <v>2794</v>
-          </cell>
-          <cell r="X11">
-            <v>2353</v>
-          </cell>
-          <cell r="Y11">
-            <v>2328</v>
-          </cell>
-        </row>
-        <row r="12">
-          <cell r="U12" t="str">
-            <v>Bird Forest Coast Park</v>
-          </cell>
-          <cell r="V12" t="str">
-            <v>Nov</v>
-          </cell>
-          <cell r="W12">
-            <v>2794</v>
-          </cell>
-          <cell r="X12">
-            <v>2327</v>
-          </cell>
-          <cell r="Y12">
-            <v>1942</v>
-          </cell>
-        </row>
-        <row r="13">
-          <cell r="U13" t="str">
-            <v>Park Photo Instagram</v>
-          </cell>
-          <cell r="V13" t="str">
-            <v>Dec</v>
-          </cell>
-          <cell r="W13">
-            <v>2813</v>
-          </cell>
-          <cell r="X13">
-            <v>2383</v>
-          </cell>
-          <cell r="Y13">
-            <v>2256</v>
-          </cell>
-        </row>
-      </sheetData>
-    </sheetDataSet>
-  </externalBook>
-</externalLink>
-</file>
-
 <file path=xl/theme/theme1.xml><?xml version="1.0" encoding="utf-8"?>
 <a:theme xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" name="Office Theme">
   <a:themeElements>
@@ -5376,9 +5152,9 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
   <dimension ref="A1:W73"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A86" workbookViewId="0">
-      <pane xSplit="2" topLeftCell="AD1" activePane="topRight" state="frozen"/>
-      <selection pane="topRight" activeCell="Z88" sqref="Z88"/>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <pane xSplit="2" topLeftCell="T1" activePane="topRight" state="frozen"/>
+      <selection pane="topRight" activeCell="S53" sqref="S53"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.35" customHeight="1"/>
@@ -5706,14 +5482,14 @@
       <c r="T5" t="s">
         <v>401</v>
       </c>
-      <c r="U5">
-        <v>4091</v>
-      </c>
-      <c r="V5">
-        <v>2379</v>
-      </c>
-      <c r="W5">
-        <v>2214</v>
+      <c r="U5" s="6">
+        <v>2296</v>
+      </c>
+      <c r="V5" s="6">
+        <v>1074</v>
+      </c>
+      <c r="W5" s="6">
+        <v>185</v>
       </c>
     </row>
     <row r="6" spans="1:23" ht="14.35" customHeight="1">
@@ -6066,7 +5842,7 @@
       <c r="I11">
         <v>33</v>
       </c>
-      <c r="J11">
+      <c r="J11" s="5">
         <v>2296</v>
       </c>
       <c r="K11" t="s">
@@ -6131,7 +5907,7 @@
       <c r="I12">
         <v>850</v>
       </c>
-      <c r="J12">
+      <c r="J12" s="5">
         <v>1074</v>
       </c>
       <c r="K12" t="s">
@@ -6196,7 +5972,7 @@
       <c r="I13">
         <v>106</v>
       </c>
-      <c r="J13">
+      <c r="J13" s="5">
         <v>185</v>
       </c>
       <c r="K13" t="s">

</xml_diff>